<commit_message>
Fix quantity of beta power switches to 0
</commit_message>
<xml_diff>
--- a/BOM/v1/ergoTHWACK v1 BOM.xlsx
+++ b/BOM/v1/ergoTHWACK v1 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\ergothwack\BOM\v1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B7D18A-86D0-4229-BB01-D9963A0A4427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F37908B-A89E-4DA4-BEF5-3E7069F6D022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{1E54C694-8349-4148-A3EA-D049736EB163}"/>
   </bookViews>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="H2" s="10">
         <f>SUM(G2:G100)</f>
-        <v>493.54999999999984</v>
+        <v>477.46999999999991</v>
       </c>
       <c r="J2" s="15"/>
       <c r="L2" s="4" t="s">
@@ -1210,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="4">
-        <f t="shared" ref="G3:G66" si="0">E3*F3</f>
+        <f t="shared" ref="G3:G45" si="0">E3*F3</f>
         <v>2.68</v>
       </c>
       <c r="H3" s="11">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="H4" s="12">
         <f>H2-H3</f>
-        <v>-117.94000000000028</v>
+        <v>-134.02000000000021</v>
       </c>
       <c r="J4" s="15"/>
       <c r="L4" s="5" t="s">
@@ -1657,11 +1657,11 @@
         <v>4.0199999999999996</v>
       </c>
       <c r="F20" s="7">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G20" s="7">
         <f t="shared" si="0"/>
-        <v>16.079999999999998</v>
+        <v>0</v>
       </c>
       <c r="J20" s="15" t="s">
         <v>173</v>
@@ -2354,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="8">
-        <f>E46*F46</f>
+        <f t="shared" ref="G46:G68" si="1">E46*F46</f>
         <v>3.88</v>
       </c>
       <c r="J46" s="15"/>
@@ -2379,7 +2379,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="8">
-        <f>E47*F47</f>
+        <f t="shared" si="1"/>
         <v>4.6500000000000004</v>
       </c>
       <c r="J47" s="15"/>
@@ -2404,7 +2404,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="8">
-        <f>E48*F48</f>
+        <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="J48" s="15"/>
@@ -2429,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="G49" s="8">
-        <f>E49*F49</f>
+        <f t="shared" si="1"/>
         <v>3.27</v>
       </c>
       <c r="J49" s="15"/>
@@ -2454,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="G50" s="8">
-        <f>E50*F50</f>
+        <f t="shared" si="1"/>
         <v>6.34</v>
       </c>
       <c r="J50" s="15"/>
@@ -2477,7 +2477,7 @@
         <v>3</v>
       </c>
       <c r="G51" s="8">
-        <f>E51*F51</f>
+        <f t="shared" si="1"/>
         <v>5.88</v>
       </c>
       <c r="J51" s="1" t="s">
@@ -2504,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="8">
-        <f>E52*F52</f>
+        <f t="shared" si="1"/>
         <v>8.59</v>
       </c>
       <c r="J52" s="15"/>
@@ -2527,7 +2527,7 @@
         <v>1</v>
       </c>
       <c r="G53" s="8">
-        <f>E53*F53</f>
+        <f t="shared" si="1"/>
         <v>19.989999999999998</v>
       </c>
       <c r="J53" s="15"/>
@@ -2550,7 +2550,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="8">
-        <f>E54*F54</f>
+        <f t="shared" si="1"/>
         <v>5.2</v>
       </c>
       <c r="J54" s="15"/>
@@ -2573,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="G55" s="8">
-        <f>E55*F55</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="J55" s="15"/>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="8">
-        <f>E56*F56</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="J56" s="15"/>
@@ -2619,7 +2619,7 @@
         <v>40</v>
       </c>
       <c r="G57" s="8">
-        <f>E57*F57</f>
+        <f t="shared" si="1"/>
         <v>3.2800000000000002</v>
       </c>
       <c r="J57" s="15"/>
@@ -2642,7 +2642,7 @@
         <v>3</v>
       </c>
       <c r="G58" s="8">
-        <f>E58*F58</f>
+        <f t="shared" si="1"/>
         <v>7.6499999999999995</v>
       </c>
       <c r="J58" s="15"/>
@@ -2665,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="8">
-        <f>E59*F59</f>
+        <f t="shared" si="1"/>
         <v>8.7200000000000006</v>
       </c>
       <c r="J59" s="15"/>
@@ -2690,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="17">
-        <f>E60*F60</f>
+        <f t="shared" si="1"/>
         <v>47.82</v>
       </c>
       <c r="J60" s="15"/>
@@ -2715,7 +2715,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="17">
-        <f>E61*F61</f>
+        <f t="shared" si="1"/>
         <v>6.42</v>
       </c>
       <c r="J61" s="15"/>
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="17">
-        <f>E62*F62</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -2764,7 +2764,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="17">
-        <f>E63*F63</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
     </row>
@@ -2788,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="G64" s="17">
-        <f>E64*F64</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
     </row>
@@ -2810,7 +2810,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="17">
-        <f>E65*F65</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -2832,7 +2832,7 @@
         <v>1</v>
       </c>
       <c r="G66" s="17">
-        <f>E66*F66</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="G67" s="17">
-        <f>E67*F67</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -2880,199 +2880,199 @@
         <v>1</v>
       </c>
       <c r="G68" s="17">
-        <f>E68*F68</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="G69">
-        <f t="shared" ref="G67:G100" si="1">E69*F69</f>
+        <f t="shared" ref="G69:G100" si="2">E69*F69</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>